<commit_message>
code cleaning and evaluation
</commit_message>
<xml_diff>
--- a/Past_results.xlsx
+++ b/Past_results.xlsx
@@ -286,15 +286,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>961920</xdr:colOff>
+      <xdr:colOff>860760</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>116280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1983240</xdr:colOff>
+      <xdr:colOff>1882080</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -307,8 +307,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13058640" y="5168160"/>
-          <a:ext cx="3259440" cy="2554920"/>
+          <a:off x="12886920" y="5168160"/>
+          <a:ext cx="3231000" cy="2554560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -323,15 +323,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>425520</xdr:colOff>
+      <xdr:colOff>324360</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>125280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>230040</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -344,8 +344,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12522240" y="2738880"/>
-          <a:ext cx="4544280" cy="1041480"/>
+          <a:off x="12350520" y="2738880"/>
+          <a:ext cx="4487040" cy="1041120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -366,9 +366,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>55440</xdr:colOff>
+      <xdr:colOff>55080</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -381,8 +381,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1918440" y="2555640"/>
-          <a:ext cx="5823360" cy="1988640"/>
+          <a:off x="1899360" y="2555640"/>
+          <a:ext cx="5747040" cy="1988280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -404,24 +404,21 @@
   </sheetPr>
   <dimension ref="B2:L11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="97.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="96.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.234693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>